<commit_message>
Sending transaction works, but on every transaction
</commit_message>
<xml_diff>
--- a/Price_contracts_grid.xlsx
+++ b/Price_contracts_grid.xlsx
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1" topLeftCell="A25">
-      <selection activeCell="C43" activeCellId="0" sqref="C43"/>
+    <sheetView workbookViewId="0" tabSelected="1" topLeftCell="A2">
+      <selection activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -944,7 +944,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="B2">
         <v>-20</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>309.5</v>
+        <v>299.9</v>
       </c>
       <c r="B3">
         <v>-19</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>309</v>
+        <v>299.8</v>
       </c>
       <c r="B4">
         <v>-18</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>308.5</v>
+        <v>299.6999999999999</v>
       </c>
       <c r="B5">
         <v>-17</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>308</v>
+        <v>299.59999999999985</v>
       </c>
       <c r="B6">
         <v>-16</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>307.5</v>
+        <v>299.4999999999998</v>
       </c>
       <c r="B7">
         <v>-15</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>307</v>
+        <v>299.3999999999997</v>
       </c>
       <c r="B8">
         <v>-14</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>306.5</v>
+        <v>299.29999999999967</v>
       </c>
       <c r="B9">
         <v>-13</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>306</v>
+        <v>299.1999999999996</v>
       </c>
       <c r="B10">
         <v>-12</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>305.5</v>
+        <v>299.0999999999995</v>
       </c>
       <c r="B11">
         <v>-11</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>305</v>
+        <v>298.9999999999995</v>
       </c>
       <c r="B12">
         <v>-10</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>304.5</v>
+        <v>298.8999999999994</v>
       </c>
       <c r="B13">
         <v>-9</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>304</v>
+        <v>298.79999999999933</v>
       </c>
       <c r="B14">
         <v>-8</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>303.5</v>
+        <v>298.6999999999993</v>
       </c>
       <c r="B15">
         <v>-7</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>303</v>
+        <v>298.5999999999992</v>
       </c>
       <c r="B16">
         <v>-6</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>302.5</v>
+        <v>298.49999999999915</v>
       </c>
       <c r="B17">
         <v>-5</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>302</v>
+        <v>298.3999999999991</v>
       </c>
       <c r="B18">
         <v>-4</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>301.5</v>
+        <v>298.29999999999905</v>
       </c>
       <c r="B19">
         <v>-3</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>301</v>
+        <v>298.19999999999897</v>
       </c>
       <c r="B20">
         <v>-2</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>300.5</v>
+        <v>298.09999999999894</v>
       </c>
       <c r="B21">
         <v>-1</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>300</v>
+        <v>297.99999999999886</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>299.5</v>
+        <v>297.8999999999988</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>299</v>
+        <v>297.79999999999876</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>298.5</v>
+        <v>297.6999999999987</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>298</v>
+        <v>297.5999999999986</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>297.5</v>
+        <v>297.4999999999986</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>297</v>
+        <v>297.3999999999985</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>296.5</v>
+        <v>297.2999999999984</v>
       </c>
       <c r="B29">
         <v>7</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>296</v>
+        <v>297.1999999999984</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>295.5</v>
+        <v>297.0999999999983</v>
       </c>
       <c r="B31">
         <v>9</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>295</v>
+        <v>296.99999999999824</v>
       </c>
       <c r="B32">
         <v>10</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>294.5</v>
+        <v>296.8999999999982</v>
       </c>
       <c r="B33">
         <v>11</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>294</v>
+        <v>296.79999999999814</v>
       </c>
       <c r="B34">
         <v>12</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>293.5</v>
+        <v>296.69999999999806</v>
       </c>
       <c r="B35">
         <v>13</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>293</v>
+        <v>296.59999999999803</v>
       </c>
       <c r="B36">
         <v>14</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>292.5</v>
+        <v>296.49999999999795</v>
       </c>
       <c r="B37">
         <v>15</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>292</v>
+        <v>296.3999999999979</v>
       </c>
       <c r="B38">
         <v>16</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>291.5</v>
+        <v>296.29999999999785</v>
       </c>
       <c r="B39">
         <v>17</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>291</v>
+        <v>296.1999999999978</v>
       </c>
       <c r="B40">
         <v>18</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>290.5</v>
+        <v>296.0999999999977</v>
       </c>
       <c r="B41">
         <v>19</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>290</v>
+        <v>295.99999999999767</v>
       </c>
       <c r="B42">
         <v>20</v>

</xml_diff>

<commit_message>
MVP - single security one-level grid bot with manual launch and no positions check
</commit_message>
<xml_diff>
--- a/Price_contracts_grid.xlsx
+++ b/Price_contracts_grid.xlsx
@@ -929,7 +929,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1" topLeftCell="A2">
-      <selection activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection activeCell="A2" activeCellId="0" sqref="A2:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -944,7 +944,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="B2">
         <v>-20</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>299.9</v>
+        <v>306.9</v>
       </c>
       <c r="B3">
         <v>-19</v>
@@ -960,7 +960,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>299.8</v>
+        <v>306.8</v>
       </c>
       <c r="B4">
         <v>-18</v>
@@ -968,7 +968,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>299.6999999999999</v>
+        <v>306.6999999999999</v>
       </c>
       <c r="B5">
         <v>-17</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>299.59999999999985</v>
+        <v>306.59999999999985</v>
       </c>
       <c r="B6">
         <v>-16</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>299.4999999999998</v>
+        <v>306.4999999999998</v>
       </c>
       <c r="B7">
         <v>-15</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>299.3999999999997</v>
+        <v>306.3999999999997</v>
       </c>
       <c r="B8">
         <v>-14</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>299.29999999999967</v>
+        <v>306.29999999999967</v>
       </c>
       <c r="B9">
         <v>-13</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>299.1999999999996</v>
+        <v>306.1999999999996</v>
       </c>
       <c r="B10">
         <v>-12</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>299.0999999999995</v>
+        <v>306.0999999999995</v>
       </c>
       <c r="B11">
         <v>-11</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>298.9999999999995</v>
+        <v>305.9999999999995</v>
       </c>
       <c r="B12">
         <v>-10</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>298.8999999999994</v>
+        <v>305.8999999999994</v>
       </c>
       <c r="B13">
         <v>-9</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>298.79999999999933</v>
+        <v>305.79999999999933</v>
       </c>
       <c r="B14">
         <v>-8</v>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>298.6999999999993</v>
+        <v>305.6999999999993</v>
       </c>
       <c r="B15">
         <v>-7</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>298.5999999999992</v>
+        <v>305.5999999999992</v>
       </c>
       <c r="B16">
         <v>-6</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>298.49999999999915</v>
+        <v>305.49999999999915</v>
       </c>
       <c r="B17">
         <v>-5</v>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>298.3999999999991</v>
+        <v>305.3999999999991</v>
       </c>
       <c r="B18">
         <v>-4</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>298.29999999999905</v>
+        <v>305.29999999999905</v>
       </c>
       <c r="B19">
         <v>-3</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>298.19999999999897</v>
+        <v>305.19999999999897</v>
       </c>
       <c r="B20">
         <v>-2</v>
@@ -1096,7 +1096,7 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>298.09999999999894</v>
+        <v>305.09999999999894</v>
       </c>
       <c r="B21">
         <v>-1</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>297.99999999999886</v>
+        <v>304.99999999999886</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>297.8999999999988</v>
+        <v>304.8999999999988</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>297.79999999999876</v>
+        <v>304.79999999999876</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>297.6999999999987</v>
+        <v>304.6999999999987</v>
       </c>
       <c r="B25">
         <v>3</v>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>297.5999999999986</v>
+        <v>304.5999999999986</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>297.4999999999986</v>
+        <v>304.4999999999986</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>297.3999999999985</v>
+        <v>304.3999999999985</v>
       </c>
       <c r="B28">
         <v>6</v>
@@ -1160,7 +1160,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>297.2999999999984</v>
+        <v>304.2999999999984</v>
       </c>
       <c r="B29">
         <v>7</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>297.1999999999984</v>
+        <v>304.1999999999984</v>
       </c>
       <c r="B30">
         <v>8</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>297.0999999999983</v>
+        <v>304.0999999999983</v>
       </c>
       <c r="B31">
         <v>9</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>296.99999999999824</v>
+        <v>303.99999999999824</v>
       </c>
       <c r="B32">
         <v>10</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>296.8999999999982</v>
+        <v>303.8999999999982</v>
       </c>
       <c r="B33">
         <v>11</v>
@@ -1200,7 +1200,7 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>296.79999999999814</v>
+        <v>303.79999999999814</v>
       </c>
       <c r="B34">
         <v>12</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>296.69999999999806</v>
+        <v>303.69999999999806</v>
       </c>
       <c r="B35">
         <v>13</v>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>296.59999999999803</v>
+        <v>303.59999999999803</v>
       </c>
       <c r="B36">
         <v>14</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>296.49999999999795</v>
+        <v>303.49999999999795</v>
       </c>
       <c r="B37">
         <v>15</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>296.3999999999979</v>
+        <v>303.3999999999979</v>
       </c>
       <c r="B38">
         <v>16</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>296.29999999999785</v>
+        <v>303.29999999999785</v>
       </c>
       <c r="B39">
         <v>17</v>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>296.1999999999978</v>
+        <v>303.1999999999978</v>
       </c>
       <c r="B40">
         <v>18</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>296.0999999999977</v>
+        <v>303.0999999999977</v>
       </c>
       <c r="B41">
         <v>19</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>295.99999999999767</v>
+        <v>302.99999999999767</v>
       </c>
       <c r="B42">
         <v>20</v>

</xml_diff>